<commit_message>
Integrate Case 3 (PDF Table extraction) into the code base
</commit_message>
<xml_diff>
--- a/workflow/python/output/covid_disparities_output_2020-05-10.xlsx
+++ b/workflow/python/output/covid_disparities_output_2020-05-10.xlsx
@@ -358,7 +358,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J10"/>
+  <dimension ref="A1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -550,22 +550,22 @@
         </is>
       </c>
       <c r="D5" t="n">
-        <v>32980</v>
+        <v>33508</v>
       </c>
       <c r="E5" t="n">
-        <v>1404</v>
+        <v>1405</v>
       </c>
       <c r="F5" t="n">
-        <v>11715</v>
+        <v>11857</v>
       </c>
       <c r="G5" t="n">
         <v>697</v>
       </c>
       <c r="H5" t="n">
-        <v>35.52</v>
+        <v>35.39</v>
       </c>
       <c r="I5" t="n">
-        <v>49.64</v>
+        <v>49.61</v>
       </c>
       <c r="J5" t="inlineStr">
         <is>
@@ -586,20 +586,20 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>5/9/2020</t>
+          <t>5/10/2020</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>46756</v>
+        <v>47138</v>
       </c>
       <c r="E6" t="n">
-        <v>4526</v>
+        <v>4551</v>
       </c>
       <c r="F6" t="n">
-        <v>14962</v>
+        <v>15084</v>
       </c>
       <c r="G6" t="n">
-        <v>1856</v>
+        <v>1866</v>
       </c>
       <c r="H6" t="n">
         <v>32</v>
@@ -750,26 +750,90 @@
         </is>
       </c>
       <c r="D10" t="n">
-        <v>3954</v>
+        <v>3981</v>
       </c>
       <c r="E10" t="n">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F10" t="n">
-        <v>1536</v>
+        <v>1544</v>
       </c>
       <c r="G10" t="n">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="H10" t="n">
-        <v>38.85</v>
+        <v>38.78</v>
       </c>
       <c r="I10" t="n">
-        <v>49.07</v>
+        <v>48.85</v>
       </c>
       <c r="J10" t="inlineStr">
         <is>
           <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="1" t="inlineStr">
+        <is>
+          <t>San Diego</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>California - San Diego</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>5/9/2020</t>
+        </is>
+      </c>
+      <c r="D11" t="n">
+        <v>4926</v>
+      </c>
+      <c r="E11" t="n">
+        <v>175</v>
+      </c>
+      <c r="F11" t="n">
+        <v>167</v>
+      </c>
+      <c r="G11" t="n">
+        <v>4</v>
+      </c>
+      <c r="H11" t="n">
+        <v>3.39</v>
+      </c>
+      <c r="I11" t="n">
+        <v>2.29</v>
+      </c>
+      <c r="J11" t="inlineStr">
+        <is>
+          <t>Success!</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="1" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Florida</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr"/>
+      <c r="D12" t="inlineStr"/>
+      <c r="E12" t="inlineStr"/>
+      <c r="F12" t="inlineStr"/>
+      <c r="G12" t="inlineStr"/>
+      <c r="H12" t="inlineStr"/>
+      <c r="I12" t="inlineStr"/>
+      <c r="J12" t="inlineStr">
+        <is>
+          <t>An error occured. ... FileNotFoundError(2, 'No such file or directory')</t>
         </is>
       </c>
     </row>

</xml_diff>